<commit_message>
Adição do icone do logo da empresa na aba do simulador
</commit_message>
<xml_diff>
--- a/Documentação/Backlog do projeto.xlsx
+++ b/Documentação/Backlog do projeto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NOMES" sheetId="2" r:id="rId1"/>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>